<commit_message>
update templete excel keprof
</commit_message>
<xml_diff>
--- a/public/assets/template/keprof.xlsx
+++ b/public/assets/template/keprof.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\pipe\public\assets\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pipe\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F8D5079-ED05-4114-853A-BD699985F619}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771BBDFF-B863-44C7-ADB2-E2240999F4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,19 +30,19 @@
     <t>name</t>
   </si>
   <si>
-    <t>kelompok</t>
-  </si>
-  <si>
-    <t>peminatan</t>
-  </si>
-  <si>
-    <t>Nama Dosen</t>
-  </si>
-  <si>
-    <t>Kelompok Peminatan</t>
-  </si>
-  <si>
-    <t>Peminatan</t>
+    <t>nim</t>
+  </si>
+  <si>
+    <t>keprofesian</t>
+  </si>
+  <si>
+    <t>NIM Mahasiswa</t>
+  </si>
+  <si>
+    <t>Nama Mahasiswa</t>
+  </si>
+  <si>
+    <t>Keprofesian</t>
   </si>
 </sst>
 </file>
@@ -363,17 +363,17 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Update All Master Data Admin, Update masterdata.py, Update template Excel Peminatan dan Keprof
</commit_message>
<xml_diff>
--- a/public/assets/template/keprof.xlsx
+++ b/public/assets/template/keprof.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pipe\public\assets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771BBDFF-B863-44C7-ADB2-E2240999F4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{337AE0D0-7808-413F-A678-EDEC3A1FA1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>nim</t>
   </si>
   <si>
-    <t>keprofesian</t>
-  </si>
-  <si>
     <t>NIM Mahasiswa</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>Keprofesian</t>
+  </si>
+  <si>
+    <t>keprof</t>
   </si>
 </sst>
 </file>
@@ -363,7 +363,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -376,18 +376,18 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>